<commit_message>
Added more scrapped data into the general dataset
</commit_message>
<xml_diff>
--- a/Data/Japanese/flower.xlsx
+++ b/Data/Japanese/flower.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julie\Documents\CuriousLine\FlowerMeaning\JapaneseMeaning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julie\Documents\CuriousLine\flower-meaning\Data\Japanese\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -4455,8 +4455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E639"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A627" workbookViewId="0">
-      <selection activeCell="F634" sqref="F634"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18:B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9301,116 +9301,166 @@
     </row>
   </sheetData>
   <mergeCells count="288">
-    <mergeCell ref="A622:A629"/>
-    <mergeCell ref="B622:B629"/>
-    <mergeCell ref="C622:C629"/>
-    <mergeCell ref="D622:D629"/>
-    <mergeCell ref="E622:E629"/>
-    <mergeCell ref="A631:A638"/>
-    <mergeCell ref="B631:B638"/>
-    <mergeCell ref="C631:C638"/>
-    <mergeCell ref="D631:D638"/>
-    <mergeCell ref="E631:E638"/>
-    <mergeCell ref="A602:A611"/>
-    <mergeCell ref="B602:B611"/>
-    <mergeCell ref="C602:C611"/>
-    <mergeCell ref="D602:D611"/>
-    <mergeCell ref="E602:E611"/>
-    <mergeCell ref="A613:A620"/>
-    <mergeCell ref="B613:B620"/>
-    <mergeCell ref="C613:C620"/>
-    <mergeCell ref="D613:D620"/>
-    <mergeCell ref="E613:E620"/>
-    <mergeCell ref="A577:A584"/>
-    <mergeCell ref="B577:B584"/>
-    <mergeCell ref="C577:C584"/>
-    <mergeCell ref="D577:D584"/>
-    <mergeCell ref="E577:E584"/>
-    <mergeCell ref="A586:A600"/>
-    <mergeCell ref="B586:B600"/>
-    <mergeCell ref="C586:C600"/>
-    <mergeCell ref="D586:D600"/>
-    <mergeCell ref="E586:E600"/>
-    <mergeCell ref="A552:A567"/>
-    <mergeCell ref="B552:B567"/>
-    <mergeCell ref="C552:C567"/>
-    <mergeCell ref="D552:D567"/>
-    <mergeCell ref="E552:E567"/>
-    <mergeCell ref="A569:A575"/>
-    <mergeCell ref="B569:B575"/>
-    <mergeCell ref="C569:C575"/>
-    <mergeCell ref="D569:D575"/>
-    <mergeCell ref="E569:E575"/>
-    <mergeCell ref="A533:A540"/>
-    <mergeCell ref="B533:B540"/>
-    <mergeCell ref="C533:C540"/>
-    <mergeCell ref="D533:D540"/>
-    <mergeCell ref="E533:E540"/>
-    <mergeCell ref="A542:A550"/>
-    <mergeCell ref="B542:B550"/>
-    <mergeCell ref="C542:C550"/>
-    <mergeCell ref="D542:D550"/>
-    <mergeCell ref="E542:E550"/>
-    <mergeCell ref="A513:A520"/>
-    <mergeCell ref="B513:B520"/>
-    <mergeCell ref="C513:C520"/>
-    <mergeCell ref="D513:D520"/>
-    <mergeCell ref="E513:E520"/>
-    <mergeCell ref="A522:A531"/>
-    <mergeCell ref="B522:B531"/>
-    <mergeCell ref="C522:C531"/>
-    <mergeCell ref="D522:D531"/>
-    <mergeCell ref="E522:E531"/>
-    <mergeCell ref="A494:A501"/>
-    <mergeCell ref="B494:B501"/>
-    <mergeCell ref="C494:C501"/>
-    <mergeCell ref="D494:D501"/>
-    <mergeCell ref="E494:E501"/>
-    <mergeCell ref="A503:A511"/>
-    <mergeCell ref="B503:B511"/>
-    <mergeCell ref="C503:C511"/>
-    <mergeCell ref="D503:D511"/>
-    <mergeCell ref="E503:E511"/>
-    <mergeCell ref="A476:A483"/>
-    <mergeCell ref="B476:B483"/>
-    <mergeCell ref="C476:C483"/>
-    <mergeCell ref="D476:D483"/>
-    <mergeCell ref="E476:E483"/>
-    <mergeCell ref="A485:A492"/>
-    <mergeCell ref="B485:B492"/>
-    <mergeCell ref="C485:C492"/>
-    <mergeCell ref="D485:D492"/>
-    <mergeCell ref="E485:E492"/>
-    <mergeCell ref="A458:A465"/>
-    <mergeCell ref="B458:B465"/>
-    <mergeCell ref="C458:C465"/>
-    <mergeCell ref="D458:D465"/>
-    <mergeCell ref="E458:E465"/>
-    <mergeCell ref="A467:A474"/>
-    <mergeCell ref="B467:B474"/>
-    <mergeCell ref="C467:C474"/>
-    <mergeCell ref="D467:D474"/>
-    <mergeCell ref="E467:E474"/>
-    <mergeCell ref="A427:A444"/>
-    <mergeCell ref="B427:B444"/>
-    <mergeCell ref="C427:C444"/>
-    <mergeCell ref="D427:D444"/>
-    <mergeCell ref="E427:E444"/>
-    <mergeCell ref="A446:A456"/>
-    <mergeCell ref="B446:B456"/>
-    <mergeCell ref="C446:C456"/>
-    <mergeCell ref="D446:D456"/>
-    <mergeCell ref="E446:E456"/>
-    <mergeCell ref="A402:A416"/>
-    <mergeCell ref="B402:B416"/>
-    <mergeCell ref="C402:C416"/>
-    <mergeCell ref="D402:D416"/>
-    <mergeCell ref="E402:E416"/>
-    <mergeCell ref="A418:A425"/>
-    <mergeCell ref="B418:B425"/>
-    <mergeCell ref="C418:C425"/>
-    <mergeCell ref="D418:D425"/>
-    <mergeCell ref="E418:E425"/>
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="B2:B8"/>
+    <mergeCell ref="C2:C8"/>
+    <mergeCell ref="D2:D8"/>
+    <mergeCell ref="E2:E8"/>
+    <mergeCell ref="A10:A16"/>
+    <mergeCell ref="B10:B16"/>
+    <mergeCell ref="C10:C16"/>
+    <mergeCell ref="D10:D16"/>
+    <mergeCell ref="E10:E16"/>
+    <mergeCell ref="A18:A32"/>
+    <mergeCell ref="B18:B32"/>
+    <mergeCell ref="C18:C32"/>
+    <mergeCell ref="D18:D32"/>
+    <mergeCell ref="E18:E32"/>
+    <mergeCell ref="A34:A48"/>
+    <mergeCell ref="B34:B48"/>
+    <mergeCell ref="C34:C48"/>
+    <mergeCell ref="D34:D48"/>
+    <mergeCell ref="E34:E48"/>
+    <mergeCell ref="A50:A60"/>
+    <mergeCell ref="B50:B60"/>
+    <mergeCell ref="C50:C60"/>
+    <mergeCell ref="D50:D60"/>
+    <mergeCell ref="E50:E60"/>
+    <mergeCell ref="A62:A78"/>
+    <mergeCell ref="B62:B78"/>
+    <mergeCell ref="C62:C78"/>
+    <mergeCell ref="D62:D78"/>
+    <mergeCell ref="E62:E78"/>
+    <mergeCell ref="A80:A86"/>
+    <mergeCell ref="B80:B86"/>
+    <mergeCell ref="C80:C86"/>
+    <mergeCell ref="D80:D86"/>
+    <mergeCell ref="E80:E86"/>
+    <mergeCell ref="A88:A95"/>
+    <mergeCell ref="B88:B95"/>
+    <mergeCell ref="C88:C95"/>
+    <mergeCell ref="D88:D95"/>
+    <mergeCell ref="E88:E95"/>
+    <mergeCell ref="A97:A104"/>
+    <mergeCell ref="B97:B104"/>
+    <mergeCell ref="C97:C104"/>
+    <mergeCell ref="D97:D104"/>
+    <mergeCell ref="E97:E104"/>
+    <mergeCell ref="A106:A115"/>
+    <mergeCell ref="B106:B115"/>
+    <mergeCell ref="C106:C115"/>
+    <mergeCell ref="D106:D115"/>
+    <mergeCell ref="E106:E115"/>
+    <mergeCell ref="A117:A131"/>
+    <mergeCell ref="B117:B131"/>
+    <mergeCell ref="C117:C131"/>
+    <mergeCell ref="D117:D131"/>
+    <mergeCell ref="E117:E131"/>
+    <mergeCell ref="A133:A146"/>
+    <mergeCell ref="B133:B146"/>
+    <mergeCell ref="C133:C146"/>
+    <mergeCell ref="D133:D146"/>
+    <mergeCell ref="E133:E146"/>
+    <mergeCell ref="A148:A155"/>
+    <mergeCell ref="B148:B155"/>
+    <mergeCell ref="C148:C155"/>
+    <mergeCell ref="D148:D155"/>
+    <mergeCell ref="E148:E155"/>
+    <mergeCell ref="A157:A164"/>
+    <mergeCell ref="B157:B164"/>
+    <mergeCell ref="C157:C164"/>
+    <mergeCell ref="D157:D164"/>
+    <mergeCell ref="E157:E164"/>
+    <mergeCell ref="A166:A173"/>
+    <mergeCell ref="B166:B173"/>
+    <mergeCell ref="C166:C173"/>
+    <mergeCell ref="D166:D173"/>
+    <mergeCell ref="E166:E173"/>
+    <mergeCell ref="A175:A184"/>
+    <mergeCell ref="B175:B184"/>
+    <mergeCell ref="C175:C184"/>
+    <mergeCell ref="D175:D184"/>
+    <mergeCell ref="E175:E184"/>
+    <mergeCell ref="A186:A193"/>
+    <mergeCell ref="B186:B193"/>
+    <mergeCell ref="C186:C193"/>
+    <mergeCell ref="D186:D193"/>
+    <mergeCell ref="E186:E193"/>
+    <mergeCell ref="A195:A204"/>
+    <mergeCell ref="B195:B204"/>
+    <mergeCell ref="C195:C204"/>
+    <mergeCell ref="D195:D204"/>
+    <mergeCell ref="E195:E204"/>
+    <mergeCell ref="A206:A216"/>
+    <mergeCell ref="B206:B216"/>
+    <mergeCell ref="C206:C216"/>
+    <mergeCell ref="D206:D216"/>
+    <mergeCell ref="E206:E216"/>
+    <mergeCell ref="A218:A225"/>
+    <mergeCell ref="B218:B225"/>
+    <mergeCell ref="C218:C225"/>
+    <mergeCell ref="D218:D225"/>
+    <mergeCell ref="E218:E225"/>
+    <mergeCell ref="A227:A241"/>
+    <mergeCell ref="B227:B241"/>
+    <mergeCell ref="C227:C241"/>
+    <mergeCell ref="D227:D241"/>
+    <mergeCell ref="E227:E241"/>
+    <mergeCell ref="A243:A250"/>
+    <mergeCell ref="B243:B250"/>
+    <mergeCell ref="C243:C250"/>
+    <mergeCell ref="D243:D250"/>
+    <mergeCell ref="E243:E250"/>
+    <mergeCell ref="A252:A259"/>
+    <mergeCell ref="B252:B259"/>
+    <mergeCell ref="C252:C259"/>
+    <mergeCell ref="D252:D259"/>
+    <mergeCell ref="E252:E259"/>
+    <mergeCell ref="A261:A268"/>
+    <mergeCell ref="B261:B268"/>
+    <mergeCell ref="C261:C268"/>
+    <mergeCell ref="D261:D268"/>
+    <mergeCell ref="E261:E268"/>
+    <mergeCell ref="A270:A280"/>
+    <mergeCell ref="B270:B280"/>
+    <mergeCell ref="C270:C280"/>
+    <mergeCell ref="D270:D280"/>
+    <mergeCell ref="E270:E280"/>
+    <mergeCell ref="A282:A295"/>
+    <mergeCell ref="B282:B295"/>
+    <mergeCell ref="C282:C295"/>
+    <mergeCell ref="D282:D295"/>
+    <mergeCell ref="E282:E295"/>
+    <mergeCell ref="A297:A304"/>
+    <mergeCell ref="B297:B304"/>
+    <mergeCell ref="C297:C304"/>
+    <mergeCell ref="D297:D304"/>
+    <mergeCell ref="E297:E304"/>
+    <mergeCell ref="A306:A312"/>
+    <mergeCell ref="B306:B312"/>
+    <mergeCell ref="C306:C312"/>
+    <mergeCell ref="D306:D312"/>
+    <mergeCell ref="E306:E312"/>
+    <mergeCell ref="A314:A328"/>
+    <mergeCell ref="B314:B328"/>
+    <mergeCell ref="C314:C328"/>
+    <mergeCell ref="D314:D328"/>
+    <mergeCell ref="E314:E328"/>
+    <mergeCell ref="A330:A337"/>
+    <mergeCell ref="B330:B337"/>
+    <mergeCell ref="C330:C337"/>
+    <mergeCell ref="D330:D337"/>
+    <mergeCell ref="E330:E337"/>
+    <mergeCell ref="A339:A346"/>
+    <mergeCell ref="B339:B346"/>
+    <mergeCell ref="C339:C346"/>
+    <mergeCell ref="D339:D346"/>
+    <mergeCell ref="E339:E346"/>
+    <mergeCell ref="A348:A355"/>
+    <mergeCell ref="B348:B355"/>
+    <mergeCell ref="C348:C355"/>
+    <mergeCell ref="D348:D355"/>
+    <mergeCell ref="E348:E355"/>
     <mergeCell ref="A384:A392"/>
     <mergeCell ref="B384:B392"/>
     <mergeCell ref="C384:C392"/>
@@ -9429,166 +9479,116 @@
     <mergeCell ref="C367:C382"/>
     <mergeCell ref="D367:D382"/>
     <mergeCell ref="E367:E382"/>
-    <mergeCell ref="A339:A346"/>
-    <mergeCell ref="B339:B346"/>
-    <mergeCell ref="C339:C346"/>
-    <mergeCell ref="D339:D346"/>
-    <mergeCell ref="E339:E346"/>
-    <mergeCell ref="A348:A355"/>
-    <mergeCell ref="B348:B355"/>
-    <mergeCell ref="C348:C355"/>
-    <mergeCell ref="D348:D355"/>
-    <mergeCell ref="E348:E355"/>
-    <mergeCell ref="A314:A328"/>
-    <mergeCell ref="B314:B328"/>
-    <mergeCell ref="C314:C328"/>
-    <mergeCell ref="D314:D328"/>
-    <mergeCell ref="E314:E328"/>
-    <mergeCell ref="A330:A337"/>
-    <mergeCell ref="B330:B337"/>
-    <mergeCell ref="C330:C337"/>
-    <mergeCell ref="D330:D337"/>
-    <mergeCell ref="E330:E337"/>
-    <mergeCell ref="A297:A304"/>
-    <mergeCell ref="B297:B304"/>
-    <mergeCell ref="C297:C304"/>
-    <mergeCell ref="D297:D304"/>
-    <mergeCell ref="E297:E304"/>
-    <mergeCell ref="A306:A312"/>
-    <mergeCell ref="B306:B312"/>
-    <mergeCell ref="C306:C312"/>
-    <mergeCell ref="D306:D312"/>
-    <mergeCell ref="E306:E312"/>
-    <mergeCell ref="A270:A280"/>
-    <mergeCell ref="B270:B280"/>
-    <mergeCell ref="C270:C280"/>
-    <mergeCell ref="D270:D280"/>
-    <mergeCell ref="E270:E280"/>
-    <mergeCell ref="A282:A295"/>
-    <mergeCell ref="B282:B295"/>
-    <mergeCell ref="C282:C295"/>
-    <mergeCell ref="D282:D295"/>
-    <mergeCell ref="E282:E295"/>
-    <mergeCell ref="A252:A259"/>
-    <mergeCell ref="B252:B259"/>
-    <mergeCell ref="C252:C259"/>
-    <mergeCell ref="D252:D259"/>
-    <mergeCell ref="E252:E259"/>
-    <mergeCell ref="A261:A268"/>
-    <mergeCell ref="B261:B268"/>
-    <mergeCell ref="C261:C268"/>
-    <mergeCell ref="D261:D268"/>
-    <mergeCell ref="E261:E268"/>
-    <mergeCell ref="A227:A241"/>
-    <mergeCell ref="B227:B241"/>
-    <mergeCell ref="C227:C241"/>
-    <mergeCell ref="D227:D241"/>
-    <mergeCell ref="E227:E241"/>
-    <mergeCell ref="A243:A250"/>
-    <mergeCell ref="B243:B250"/>
-    <mergeCell ref="C243:C250"/>
-    <mergeCell ref="D243:D250"/>
-    <mergeCell ref="E243:E250"/>
-    <mergeCell ref="A206:A216"/>
-    <mergeCell ref="B206:B216"/>
-    <mergeCell ref="C206:C216"/>
-    <mergeCell ref="D206:D216"/>
-    <mergeCell ref="E206:E216"/>
-    <mergeCell ref="A218:A225"/>
-    <mergeCell ref="B218:B225"/>
-    <mergeCell ref="C218:C225"/>
-    <mergeCell ref="D218:D225"/>
-    <mergeCell ref="E218:E225"/>
-    <mergeCell ref="A186:A193"/>
-    <mergeCell ref="B186:B193"/>
-    <mergeCell ref="C186:C193"/>
-    <mergeCell ref="D186:D193"/>
-    <mergeCell ref="E186:E193"/>
-    <mergeCell ref="A195:A204"/>
-    <mergeCell ref="B195:B204"/>
-    <mergeCell ref="C195:C204"/>
-    <mergeCell ref="D195:D204"/>
-    <mergeCell ref="E195:E204"/>
-    <mergeCell ref="A166:A173"/>
-    <mergeCell ref="B166:B173"/>
-    <mergeCell ref="C166:C173"/>
-    <mergeCell ref="D166:D173"/>
-    <mergeCell ref="E166:E173"/>
-    <mergeCell ref="A175:A184"/>
-    <mergeCell ref="B175:B184"/>
-    <mergeCell ref="C175:C184"/>
-    <mergeCell ref="D175:D184"/>
-    <mergeCell ref="E175:E184"/>
-    <mergeCell ref="A148:A155"/>
-    <mergeCell ref="B148:B155"/>
-    <mergeCell ref="C148:C155"/>
-    <mergeCell ref="D148:D155"/>
-    <mergeCell ref="E148:E155"/>
-    <mergeCell ref="A157:A164"/>
-    <mergeCell ref="B157:B164"/>
-    <mergeCell ref="C157:C164"/>
-    <mergeCell ref="D157:D164"/>
-    <mergeCell ref="E157:E164"/>
-    <mergeCell ref="A117:A131"/>
-    <mergeCell ref="B117:B131"/>
-    <mergeCell ref="C117:C131"/>
-    <mergeCell ref="D117:D131"/>
-    <mergeCell ref="E117:E131"/>
-    <mergeCell ref="A133:A146"/>
-    <mergeCell ref="B133:B146"/>
-    <mergeCell ref="C133:C146"/>
-    <mergeCell ref="D133:D146"/>
-    <mergeCell ref="E133:E146"/>
-    <mergeCell ref="A97:A104"/>
-    <mergeCell ref="B97:B104"/>
-    <mergeCell ref="C97:C104"/>
-    <mergeCell ref="D97:D104"/>
-    <mergeCell ref="E97:E104"/>
-    <mergeCell ref="A106:A115"/>
-    <mergeCell ref="B106:B115"/>
-    <mergeCell ref="C106:C115"/>
-    <mergeCell ref="D106:D115"/>
-    <mergeCell ref="E106:E115"/>
-    <mergeCell ref="A80:A86"/>
-    <mergeCell ref="B80:B86"/>
-    <mergeCell ref="C80:C86"/>
-    <mergeCell ref="D80:D86"/>
-    <mergeCell ref="E80:E86"/>
-    <mergeCell ref="A88:A95"/>
-    <mergeCell ref="B88:B95"/>
-    <mergeCell ref="C88:C95"/>
-    <mergeCell ref="D88:D95"/>
-    <mergeCell ref="E88:E95"/>
-    <mergeCell ref="A50:A60"/>
-    <mergeCell ref="B50:B60"/>
-    <mergeCell ref="C50:C60"/>
-    <mergeCell ref="D50:D60"/>
-    <mergeCell ref="E50:E60"/>
-    <mergeCell ref="A62:A78"/>
-    <mergeCell ref="B62:B78"/>
-    <mergeCell ref="C62:C78"/>
-    <mergeCell ref="D62:D78"/>
-    <mergeCell ref="E62:E78"/>
-    <mergeCell ref="A18:A32"/>
-    <mergeCell ref="B18:B32"/>
-    <mergeCell ref="C18:C32"/>
-    <mergeCell ref="D18:D32"/>
-    <mergeCell ref="E18:E32"/>
-    <mergeCell ref="A34:A48"/>
-    <mergeCell ref="B34:B48"/>
-    <mergeCell ref="C34:C48"/>
-    <mergeCell ref="D34:D48"/>
-    <mergeCell ref="E34:E48"/>
-    <mergeCell ref="A2:A8"/>
-    <mergeCell ref="B2:B8"/>
-    <mergeCell ref="C2:C8"/>
-    <mergeCell ref="D2:D8"/>
-    <mergeCell ref="E2:E8"/>
-    <mergeCell ref="A10:A16"/>
-    <mergeCell ref="B10:B16"/>
-    <mergeCell ref="C10:C16"/>
-    <mergeCell ref="D10:D16"/>
-    <mergeCell ref="E10:E16"/>
+    <mergeCell ref="A402:A416"/>
+    <mergeCell ref="B402:B416"/>
+    <mergeCell ref="C402:C416"/>
+    <mergeCell ref="D402:D416"/>
+    <mergeCell ref="E402:E416"/>
+    <mergeCell ref="A418:A425"/>
+    <mergeCell ref="B418:B425"/>
+    <mergeCell ref="C418:C425"/>
+    <mergeCell ref="D418:D425"/>
+    <mergeCell ref="E418:E425"/>
+    <mergeCell ref="A427:A444"/>
+    <mergeCell ref="B427:B444"/>
+    <mergeCell ref="C427:C444"/>
+    <mergeCell ref="D427:D444"/>
+    <mergeCell ref="E427:E444"/>
+    <mergeCell ref="A446:A456"/>
+    <mergeCell ref="B446:B456"/>
+    <mergeCell ref="C446:C456"/>
+    <mergeCell ref="D446:D456"/>
+    <mergeCell ref="E446:E456"/>
+    <mergeCell ref="A458:A465"/>
+    <mergeCell ref="B458:B465"/>
+    <mergeCell ref="C458:C465"/>
+    <mergeCell ref="D458:D465"/>
+    <mergeCell ref="E458:E465"/>
+    <mergeCell ref="A467:A474"/>
+    <mergeCell ref="B467:B474"/>
+    <mergeCell ref="C467:C474"/>
+    <mergeCell ref="D467:D474"/>
+    <mergeCell ref="E467:E474"/>
+    <mergeCell ref="A476:A483"/>
+    <mergeCell ref="B476:B483"/>
+    <mergeCell ref="C476:C483"/>
+    <mergeCell ref="D476:D483"/>
+    <mergeCell ref="E476:E483"/>
+    <mergeCell ref="A485:A492"/>
+    <mergeCell ref="B485:B492"/>
+    <mergeCell ref="C485:C492"/>
+    <mergeCell ref="D485:D492"/>
+    <mergeCell ref="E485:E492"/>
+    <mergeCell ref="A494:A501"/>
+    <mergeCell ref="B494:B501"/>
+    <mergeCell ref="C494:C501"/>
+    <mergeCell ref="D494:D501"/>
+    <mergeCell ref="E494:E501"/>
+    <mergeCell ref="A503:A511"/>
+    <mergeCell ref="B503:B511"/>
+    <mergeCell ref="C503:C511"/>
+    <mergeCell ref="D503:D511"/>
+    <mergeCell ref="E503:E511"/>
+    <mergeCell ref="A513:A520"/>
+    <mergeCell ref="B513:B520"/>
+    <mergeCell ref="C513:C520"/>
+    <mergeCell ref="D513:D520"/>
+    <mergeCell ref="E513:E520"/>
+    <mergeCell ref="A522:A531"/>
+    <mergeCell ref="B522:B531"/>
+    <mergeCell ref="C522:C531"/>
+    <mergeCell ref="D522:D531"/>
+    <mergeCell ref="E522:E531"/>
+    <mergeCell ref="A533:A540"/>
+    <mergeCell ref="B533:B540"/>
+    <mergeCell ref="C533:C540"/>
+    <mergeCell ref="D533:D540"/>
+    <mergeCell ref="E533:E540"/>
+    <mergeCell ref="A542:A550"/>
+    <mergeCell ref="B542:B550"/>
+    <mergeCell ref="C542:C550"/>
+    <mergeCell ref="D542:D550"/>
+    <mergeCell ref="E542:E550"/>
+    <mergeCell ref="A552:A567"/>
+    <mergeCell ref="B552:B567"/>
+    <mergeCell ref="C552:C567"/>
+    <mergeCell ref="D552:D567"/>
+    <mergeCell ref="E552:E567"/>
+    <mergeCell ref="A569:A575"/>
+    <mergeCell ref="B569:B575"/>
+    <mergeCell ref="C569:C575"/>
+    <mergeCell ref="D569:D575"/>
+    <mergeCell ref="E569:E575"/>
+    <mergeCell ref="A577:A584"/>
+    <mergeCell ref="B577:B584"/>
+    <mergeCell ref="C577:C584"/>
+    <mergeCell ref="D577:D584"/>
+    <mergeCell ref="E577:E584"/>
+    <mergeCell ref="A586:A600"/>
+    <mergeCell ref="B586:B600"/>
+    <mergeCell ref="C586:C600"/>
+    <mergeCell ref="D586:D600"/>
+    <mergeCell ref="E586:E600"/>
+    <mergeCell ref="A602:A611"/>
+    <mergeCell ref="B602:B611"/>
+    <mergeCell ref="C602:C611"/>
+    <mergeCell ref="D602:D611"/>
+    <mergeCell ref="E602:E611"/>
+    <mergeCell ref="A613:A620"/>
+    <mergeCell ref="B613:B620"/>
+    <mergeCell ref="C613:C620"/>
+    <mergeCell ref="D613:D620"/>
+    <mergeCell ref="E613:E620"/>
+    <mergeCell ref="A622:A629"/>
+    <mergeCell ref="B622:B629"/>
+    <mergeCell ref="C622:C629"/>
+    <mergeCell ref="D622:D629"/>
+    <mergeCell ref="E622:E629"/>
+    <mergeCell ref="A631:A638"/>
+    <mergeCell ref="B631:B638"/>
+    <mergeCell ref="C631:C638"/>
+    <mergeCell ref="D631:D638"/>
+    <mergeCell ref="E631:E638"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1" tooltip="Romaji" display="https://en.wikipedia.org/wiki/Romaji"/>

</xml_diff>